<commit_message>
rerun results with correct imputation for Age first drink
</commit_message>
<xml_diff>
--- a/post_hoc_milena/Confounds_list_Milena_v4.xlsx
+++ b/post_hoc_milena/Confounds_list_Milena_v4.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roshanrane/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musialm\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C217CB5-F9CA-FB44-8A20-C6EE601E0FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24260" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24260" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,13 +34,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Microsoft Office User</author>
     <author>Rane, Roshan Prakash</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -64,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="E1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="J1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1018,7 +1017,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1108,8 +1107,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1420,14 +1419,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:XFD39"/>
+    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="4" width="25.83203125" customWidth="1"/>
     <col min="5" max="5" width="22.1640625" customWidth="1"/>
@@ -1438,7 +1437,7 @@
     <col min="10" max="10" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1470,7 +1469,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1498,7 +1497,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1526,7 +1525,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1554,7 +1553,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1582,7 +1581,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1610,7 +1609,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1638,7 +1637,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1666,7 +1665,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1694,7 +1693,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1722,7 +1721,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1750,7 +1749,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1778,7 +1777,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1806,7 +1805,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1834,7 +1833,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1862,7 +1861,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1890,7 +1889,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1918,7 +1917,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1946,7 +1945,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1974,7 +1973,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -2002,7 +2001,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -2030,7 +2029,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -2058,7 +2057,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -2086,7 +2085,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -2114,7 +2113,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -2133,7 +2132,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>15</v>
@@ -2142,7 +2141,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2170,7 +2169,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2198,7 +2197,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -2226,7 +2225,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -2254,7 +2253,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -2282,7 +2281,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -2310,7 +2309,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -2338,7 +2337,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -2366,7 +2365,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -2398,7 +2397,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -2430,7 +2429,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2462,7 +2461,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -2494,7 +2493,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -2526,7 +2525,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -2558,7 +2557,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -2590,7 +2589,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -2622,7 +2621,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -2650,7 +2649,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -2678,7 +2677,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2706,7 +2705,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -2734,7 +2733,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -2762,7 +2761,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -2790,7 +2789,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -2818,7 +2817,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -2846,7 +2845,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -2874,7 +2873,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -2902,7 +2901,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -2930,7 +2929,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -2958,7 +2957,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -2986,7 +2985,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -3014,7 +3013,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -3046,7 +3045,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>10</v>
       </c>
@@ -3078,7 +3077,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -3110,7 +3109,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>10</v>
       </c>
@@ -3142,7 +3141,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -3174,7 +3173,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>10</v>
       </c>
@@ -3206,7 +3205,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -3238,7 +3237,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -3270,7 +3269,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -3302,7 +3301,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -3334,7 +3333,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>10</v>
       </c>
@@ -3366,7 +3365,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -3398,7 +3397,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -3430,7 +3429,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>10</v>
       </c>
@@ -3462,7 +3461,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>10</v>
       </c>
@@ -3494,7 +3493,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>10</v>
       </c>
@@ -3526,7 +3525,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>10</v>
       </c>
@@ -3558,7 +3557,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -3593,7 +3592,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="255" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" ht="232.5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>10</v>
       </c>
@@ -3625,7 +3624,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="153" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>10</v>
       </c>
@@ -3657,7 +3656,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>10</v>
       </c>
@@ -3685,7 +3684,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>10</v>
       </c>
@@ -3713,7 +3712,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>10</v>
       </c>
@@ -3741,7 +3740,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="204" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>10</v>
       </c>
@@ -3773,7 +3772,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>10</v>
       </c>
@@ -3801,7 +3800,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>10</v>
       </c>
@@ -3829,7 +3828,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="119" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>10</v>
       </c>
@@ -3861,7 +3860,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>10</v>
       </c>
@@ -3889,7 +3888,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>10</v>
       </c>
@@ -3917,7 +3916,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>10</v>
       </c>
@@ -3945,7 +3944,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>10</v>
       </c>
@@ -3973,7 +3972,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>10</v>
       </c>
@@ -4001,7 +4000,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>10</v>
       </c>
@@ -4029,7 +4028,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>10</v>
       </c>
@@ -4057,7 +4056,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>10</v>
       </c>
@@ -4085,7 +4084,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>10</v>
       </c>
@@ -4113,7 +4112,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>10</v>
       </c>
@@ -4141,7 +4140,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>10</v>
       </c>
@@ -4169,7 +4168,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>10</v>
       </c>
@@ -4197,7 +4196,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>10</v>
       </c>
@@ -4229,7 +4228,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>10</v>
       </c>
@@ -4261,7 +4260,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>10</v>
       </c>
@@ -4293,7 +4292,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>10</v>
       </c>
@@ -4325,7 +4324,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>10</v>
       </c>
@@ -4357,7 +4356,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>10</v>
       </c>
@@ -4385,7 +4384,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>10</v>
       </c>
@@ -4413,7 +4412,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>10</v>
       </c>
@@ -4441,7 +4440,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>10</v>
       </c>
@@ -4469,7 +4468,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>10</v>
       </c>
@@ -4497,7 +4496,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>10</v>
       </c>
@@ -4525,7 +4524,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>10</v>
       </c>
@@ -4553,7 +4552,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>10</v>
       </c>
@@ -4581,7 +4580,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>10</v>
       </c>
@@ -4609,7 +4608,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>10</v>
       </c>
@@ -4637,7 +4636,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>10</v>
       </c>
@@ -4665,7 +4664,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>10</v>
       </c>
@@ -4693,7 +4692,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>10</v>
       </c>
@@ -4721,7 +4720,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>10</v>
       </c>
@@ -4749,7 +4748,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>10</v>
       </c>
@@ -4777,7 +4776,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>10</v>
       </c>
@@ -4805,7 +4804,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>10</v>
       </c>
@@ -4833,7 +4832,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>10</v>
       </c>
@@ -4861,7 +4860,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>10</v>
       </c>
@@ -4893,7 +4892,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>10</v>
       </c>
@@ -4925,7 +4924,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>233</v>
       </c>
@@ -4953,7 +4952,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>233</v>
       </c>
@@ -4985,7 +4984,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>233</v>
       </c>
@@ -5017,7 +5016,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>233</v>
       </c>
@@ -5049,7 +5048,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>233</v>
       </c>
@@ -5081,7 +5080,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>233</v>
       </c>
@@ -5113,7 +5112,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>233</v>
       </c>
@@ -5145,7 +5144,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>233</v>
       </c>
@@ -5177,7 +5176,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>233</v>
       </c>
@@ -5209,7 +5208,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>233</v>
       </c>
@@ -5241,7 +5240,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>233</v>
       </c>
@@ -5273,7 +5272,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>233</v>
       </c>
@@ -5305,7 +5304,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>233</v>
       </c>
@@ -5337,7 +5336,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>233</v>
       </c>
@@ -5371,7 +5370,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K73" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K73" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
all results of causal0 are uploaded for reproducibility
</commit_message>
<xml_diff>
--- a/post_hoc_milena/Confounds_list_Milena_v4.xlsx
+++ b/post_hoc_milena/Confounds_list_Milena_v4.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musialm\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roshanrane/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B66E02-A375-FA42-B883-1E399D093EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24260" windowHeight="16000"/>
+    <workbookView xWindow="41380" yWindow="-440" windowWidth="24260" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,28 +20,18 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
     <author>Rane, Roshan Prakash</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -63,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="1" shapeId="0">
+    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -78,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -101,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -124,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="1" shapeId="0">
+    <comment ref="J1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -1017,7 +1008,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1060,11 +1051,13 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1107,8 +1100,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1419,14 +1412,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="4" width="25.83203125" customWidth="1"/>
     <col min="5" max="5" width="22.1640625" customWidth="1"/>
@@ -1437,7 +1430,7 @@
     <col min="10" max="10" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1469,7 +1462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1497,7 +1490,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1525,7 +1518,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1553,7 +1546,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1581,7 +1574,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1609,7 +1602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1637,7 +1630,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1665,7 +1658,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1693,7 +1686,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1721,7 +1714,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1749,7 +1742,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1777,7 +1770,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1805,7 +1798,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1833,7 +1826,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1861,7 +1854,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1889,7 +1882,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1917,7 +1910,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1945,7 +1938,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1973,7 +1966,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -2001,7 +1994,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -2029,7 +2022,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -2057,7 +2050,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -2085,7 +2078,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -2113,7 +2106,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -2141,7 +2134,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2169,7 +2162,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2197,7 +2190,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -2225,7 +2218,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -2244,7 +2237,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>15</v>
@@ -2253,7 +2246,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -2272,7 +2265,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>15</v>
@@ -2281,7 +2274,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -2300,7 +2293,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>15</v>
@@ -2309,7 +2302,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -2328,7 +2321,7 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>15</v>
@@ -2337,7 +2330,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -2356,7 +2349,7 @@
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>15</v>
@@ -2365,7 +2358,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -2388,7 +2381,7 @@
         <v>93</v>
       </c>
       <c r="H34" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>15</v>
@@ -2397,7 +2390,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -2420,7 +2413,7 @@
         <v>99</v>
       </c>
       <c r="H35" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>15</v>
@@ -2429,7 +2422,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2452,7 +2445,7 @@
         <v>103</v>
       </c>
       <c r="H36" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I36" s="4" t="s">
         <v>15</v>
@@ -2461,7 +2454,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -2493,7 +2486,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -2525,7 +2518,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -2557,7 +2550,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -2589,7 +2582,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -2621,7 +2614,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -2649,7 +2642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -2677,7 +2670,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2705,7 +2698,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -2733,7 +2726,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -2761,7 +2754,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -2789,7 +2782,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -2817,7 +2810,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -2836,7 +2829,7 @@
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
       <c r="H49" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49" s="4" t="s">
         <v>15</v>
@@ -2845,7 +2838,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -2864,7 +2857,7 @@
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" s="4" t="s">
         <v>15</v>
@@ -2873,7 +2866,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -2892,7 +2885,7 @@
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" s="4" t="s">
         <v>15</v>
@@ -2901,7 +2894,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -2920,7 +2913,7 @@
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52" s="4" t="s">
         <v>15</v>
@@ -2929,7 +2922,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -2957,7 +2950,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -2985,7 +2978,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -3013,7 +3006,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -3045,7 +3038,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>10</v>
       </c>
@@ -3077,7 +3070,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -3109,7 +3102,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>10</v>
       </c>
@@ -3141,7 +3134,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -3173,7 +3166,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>10</v>
       </c>
@@ -3205,7 +3198,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -3237,7 +3230,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -3269,7 +3262,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -3301,7 +3294,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -3324,7 +3317,7 @@
         <v>134</v>
       </c>
       <c r="H65" s="4">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="I65" s="4" t="s">
         <v>15</v>
@@ -3333,7 +3326,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>10</v>
       </c>
@@ -3365,7 +3358,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -3397,7 +3390,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -3429,7 +3422,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>10</v>
       </c>
@@ -3461,7 +3454,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>10</v>
       </c>
@@ -3493,7 +3486,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>10</v>
       </c>
@@ -3525,7 +3518,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>10</v>
       </c>
@@ -3557,7 +3550,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -3592,7 +3585,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="232.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>10</v>
       </c>
@@ -3624,7 +3617,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" ht="153" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>10</v>
       </c>
@@ -3656,7 +3649,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>10</v>
       </c>
@@ -3675,7 +3668,7 @@
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
       <c r="H76" s="4">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="I76" s="4" t="s">
         <v>15</v>
@@ -3684,7 +3677,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>10</v>
       </c>
@@ -3703,7 +3696,7 @@
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
       <c r="H77" s="4">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="I77" s="4" t="s">
         <v>15</v>
@@ -3712,7 +3705,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>10</v>
       </c>
@@ -3740,7 +3733,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="170.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" ht="204" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>10</v>
       </c>
@@ -3763,7 +3756,7 @@
         <v>178</v>
       </c>
       <c r="H79" s="4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I79" s="4" t="s">
         <v>15</v>
@@ -3772,7 +3765,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>10</v>
       </c>
@@ -3800,7 +3793,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>10</v>
       </c>
@@ -3828,7 +3821,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>10</v>
       </c>
@@ -3860,7 +3853,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>10</v>
       </c>
@@ -3888,7 +3881,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>10</v>
       </c>
@@ -3916,7 +3909,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>10</v>
       </c>
@@ -3944,7 +3937,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>10</v>
       </c>
@@ -3972,7 +3965,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>10</v>
       </c>
@@ -4000,7 +3993,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>10</v>
       </c>
@@ -4028,7 +4021,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>10</v>
       </c>
@@ -4056,7 +4049,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>10</v>
       </c>
@@ -4084,7 +4077,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>10</v>
       </c>
@@ -4112,7 +4105,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>10</v>
       </c>
@@ -4140,7 +4133,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>10</v>
       </c>
@@ -4159,7 +4152,7 @@
       <c r="F93" s="4"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I93" s="4" t="s">
         <v>15</v>
@@ -4168,7 +4161,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>10</v>
       </c>
@@ -4187,7 +4180,7 @@
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
       <c r="H94" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I94" s="4" t="s">
         <v>15</v>
@@ -4196,7 +4189,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>10</v>
       </c>
@@ -4228,7 +4221,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>10</v>
       </c>
@@ -4251,7 +4244,7 @@
         <v>221</v>
       </c>
       <c r="H96" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I96" s="4" t="s">
         <v>15</v>
@@ -4260,7 +4253,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>10</v>
       </c>
@@ -4292,7 +4285,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>10</v>
       </c>
@@ -4324,7 +4317,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>10</v>
       </c>
@@ -4356,7 +4349,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>10</v>
       </c>
@@ -4375,7 +4368,7 @@
       <c r="F100" s="4"/>
       <c r="G100" s="4"/>
       <c r="H100" s="4">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I100" s="4" t="s">
         <v>15</v>
@@ -4384,7 +4377,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>10</v>
       </c>
@@ -4412,7 +4405,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>10</v>
       </c>
@@ -4440,7 +4433,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>10</v>
       </c>
@@ -4468,7 +4461,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>10</v>
       </c>
@@ -4496,7 +4489,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>10</v>
       </c>
@@ -4524,7 +4517,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>10</v>
       </c>
@@ -4552,7 +4545,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>10</v>
       </c>
@@ -4580,7 +4573,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>10</v>
       </c>
@@ -4608,7 +4601,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>10</v>
       </c>
@@ -4636,7 +4629,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>10</v>
       </c>
@@ -4664,7 +4657,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>10</v>
       </c>
@@ -4692,7 +4685,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>10</v>
       </c>
@@ -4720,7 +4713,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>10</v>
       </c>
@@ -4748,7 +4741,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>10</v>
       </c>
@@ -4776,7 +4769,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>10</v>
       </c>
@@ -4804,7 +4797,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>10</v>
       </c>
@@ -4832,7 +4825,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>10</v>
       </c>
@@ -4860,7 +4853,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>10</v>
       </c>
@@ -4883,7 +4876,7 @@
         <v>99</v>
       </c>
       <c r="H118" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I118" s="4" t="s">
         <v>15</v>
@@ -4892,7 +4885,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>10</v>
       </c>
@@ -4915,7 +4908,7 @@
         <v>103</v>
       </c>
       <c r="H119" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I119" s="4" t="s">
         <v>15</v>
@@ -4924,7 +4917,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>233</v>
       </c>
@@ -4952,7 +4945,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>233</v>
       </c>
@@ -4984,7 +4977,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>233</v>
       </c>
@@ -5016,7 +5009,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>233</v>
       </c>
@@ -5048,7 +5041,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>233</v>
       </c>
@@ -5080,7 +5073,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>233</v>
       </c>
@@ -5112,7 +5105,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>233</v>
       </c>
@@ -5144,7 +5137,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>233</v>
       </c>
@@ -5176,7 +5169,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>233</v>
       </c>
@@ -5199,7 +5192,7 @@
         <v>269</v>
       </c>
       <c r="H128" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I128" s="4" t="s">
         <v>15</v>
@@ -5208,7 +5201,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>233</v>
       </c>
@@ -5231,7 +5224,7 @@
         <v>272</v>
       </c>
       <c r="H129" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I129" s="4" t="s">
         <v>15</v>
@@ -5240,7 +5233,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>233</v>
       </c>
@@ -5272,7 +5265,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>233</v>
       </c>
@@ -5304,7 +5297,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>233</v>
       </c>
@@ -5336,7 +5329,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>233</v>
       </c>
@@ -5370,7 +5363,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K73" r:id="rId1"/>
+    <hyperlink ref="K73" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>